<commit_message>
updated basic nursing script
</commit_message>
<xml_diff>
--- a/EXAMS_INTERNAL/ND/ND-COURSES/course-code-creditUnit.xlsx
+++ b/EXAMS_INTERNAL/ND/ND-COURSES/course-code-creditUnit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="19140" windowHeight="7090" firstSheet="2" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="140" windowWidth="19140" windowHeight="7090" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ND-FIRST-YEAR-FIRST-SEMESTER" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t>COURSE CODE</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>Community Based Clinical Practice</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Hospital Based Clinical Practice</t>
@@ -641,7 +638,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -652,7 +649,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -663,7 +660,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -674,7 +671,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -685,7 +682,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -696,7 +693,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -707,7 +704,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -718,7 +715,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -740,7 +737,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -759,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -783,7 +780,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -794,7 +791,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -805,7 +802,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -816,7 +813,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -827,7 +824,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -838,7 +835,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -849,7 +846,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -860,7 +857,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -902,7 +899,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -913,7 +910,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -924,7 +921,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -935,7 +932,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -946,7 +943,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -957,7 +954,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -968,7 +965,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -979,7 +976,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -990,7 +987,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1001,7 +998,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
@@ -1019,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1043,7 +1040,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -1054,7 +1051,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1065,7 +1062,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -1076,7 +1073,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -1087,7 +1084,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -1098,7 +1095,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -1109,7 +1106,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -1120,7 +1117,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -1131,7 +1128,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
@@ -1142,7 +1139,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
@@ -1153,24 +1150,24 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
-        <v>44</v>
+      <c r="C12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
         <v>44</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>